<commit_message>
modify data augmentation results
</commit_message>
<xml_diff>
--- a/aug_pc_result/2026_Feb_06_11_23_22_d_separation_kci_pc_gt_graph_AdaSyn_20_3001859/aug_pc_raw_eval_res.xlsx
+++ b/aug_pc_result/2026_Feb_06_11_23_22_d_separation_kci_pc_gt_graph_AdaSyn_20_3001859/aug_pc_raw_eval_res.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CausalLearning\code\aug_pc_result\2026_Feb_06_11_23_22_d_separation_kci_pc_gt_graph_AdaSyn_20_3001859\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D8A4CE-A9CD-4C5A-A502-68F619C6BFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0057673E-6DA8-454F-94AB-313964F9949E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AD$513</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -514,10 +517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AD513"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A475" workbookViewId="0">
-      <selection activeCell="AD2" sqref="A2:AD513"/>
+    <sheetView tabSelected="1" topLeftCell="F437" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131:AD513"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -614,7 +618,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -706,7 +710,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -798,7 +802,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -890,7 +894,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -982,7 +986,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1074,7 +1078,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1166,7 +1170,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1258,7 +1262,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1350,7 +1354,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1442,7 +1446,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1534,7 +1538,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1626,7 +1630,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1718,7 +1722,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1810,7 +1814,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1902,7 +1906,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1994,7 +1998,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2086,7 +2090,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -2178,7 +2182,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -2270,7 +2274,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -2362,7 +2366,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -2454,7 +2458,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -2546,7 +2550,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -2638,7 +2642,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -2730,7 +2734,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -2822,7 +2826,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2914,7 +2918,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -3006,7 +3010,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -3098,7 +3102,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -3190,7 +3194,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -3282,7 +3286,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -3374,7 +3378,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -3466,7 +3470,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -3558,7 +3562,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -3650,7 +3654,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -3742,7 +3746,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -3834,7 +3838,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -3926,7 +3930,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -4018,7 +4022,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -4110,7 +4114,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -4202,7 +4206,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>30</v>
       </c>
@@ -4294,7 +4298,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -4386,7 +4390,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -4478,7 +4482,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>30</v>
       </c>
@@ -4570,7 +4574,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>30</v>
       </c>
@@ -4662,7 +4666,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>30</v>
       </c>
@@ -4754,7 +4758,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -4846,7 +4850,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>30</v>
       </c>
@@ -4938,7 +4942,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>30</v>
       </c>
@@ -5030,7 +5034,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -5122,7 +5126,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>30</v>
       </c>
@@ -5214,7 +5218,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>30</v>
       </c>
@@ -5306,7 +5310,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>30</v>
       </c>
@@ -5398,7 +5402,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>30</v>
       </c>
@@ -5490,7 +5494,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>30</v>
       </c>
@@ -5582,7 +5586,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>30</v>
       </c>
@@ -5674,7 +5678,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>30</v>
       </c>
@@ -5766,7 +5770,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>30</v>
       </c>
@@ -5858,7 +5862,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>30</v>
       </c>
@@ -5950,7 +5954,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>30</v>
       </c>
@@ -6042,7 +6046,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>30</v>
       </c>
@@ -6134,7 +6138,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>30</v>
       </c>
@@ -6226,7 +6230,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>30</v>
       </c>
@@ -6318,7 +6322,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>30</v>
       </c>
@@ -6410,7 +6414,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>30</v>
       </c>
@@ -6502,7 +6506,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>30</v>
       </c>
@@ -6594,7 +6598,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>30</v>
       </c>
@@ -6686,7 +6690,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>30</v>
       </c>
@@ -6778,7 +6782,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>30</v>
       </c>
@@ -6870,7 +6874,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>30</v>
       </c>
@@ -6962,7 +6966,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>30</v>
       </c>
@@ -7054,7 +7058,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>30</v>
       </c>
@@ -7146,7 +7150,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>30</v>
       </c>
@@ -7238,7 +7242,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>30</v>
       </c>
@@ -7330,7 +7334,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>30</v>
       </c>
@@ -7422,7 +7426,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>30</v>
       </c>
@@ -7514,7 +7518,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>30</v>
       </c>
@@ -7606,7 +7610,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>30</v>
       </c>
@@ -7698,7 +7702,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>30</v>
       </c>
@@ -7790,7 +7794,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>30</v>
       </c>
@@ -7882,7 +7886,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>30</v>
       </c>
@@ -7974,7 +7978,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="82" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>30</v>
       </c>
@@ -8066,7 +8070,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>30</v>
       </c>
@@ -8158,7 +8162,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="84" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>30</v>
       </c>
@@ -8250,7 +8254,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="85" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>30</v>
       </c>
@@ -8342,7 +8346,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="86" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>30</v>
       </c>
@@ -8434,7 +8438,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="87" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>30</v>
       </c>
@@ -8526,7 +8530,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="88" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>30</v>
       </c>
@@ -8618,7 +8622,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>30</v>
       </c>
@@ -8710,7 +8714,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>30</v>
       </c>
@@ -8802,7 +8806,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="91" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>30</v>
       </c>
@@ -8894,7 +8898,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="92" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>30</v>
       </c>
@@ -8986,7 +8990,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="93" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>30</v>
       </c>
@@ -9078,7 +9082,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="94" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>30</v>
       </c>
@@ -9170,7 +9174,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="95" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>30</v>
       </c>
@@ -9262,7 +9266,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="96" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>30</v>
       </c>
@@ -9354,7 +9358,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>30</v>
       </c>
@@ -9446,7 +9450,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>30</v>
       </c>
@@ -9538,7 +9542,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="99" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>30</v>
       </c>
@@ -9630,7 +9634,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>30</v>
       </c>
@@ -9722,7 +9726,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="101" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>30</v>
       </c>
@@ -9814,7 +9818,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="102" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>30</v>
       </c>
@@ -9906,7 +9910,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>30</v>
       </c>
@@ -9998,7 +10002,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="104" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>30</v>
       </c>
@@ -10090,7 +10094,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="105" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>30</v>
       </c>
@@ -10182,7 +10186,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="106" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>30</v>
       </c>
@@ -10274,7 +10278,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>30</v>
       </c>
@@ -10366,7 +10370,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="108" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>30</v>
       </c>
@@ -10458,7 +10462,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="109" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>30</v>
       </c>
@@ -10550,7 +10554,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="110" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>30</v>
       </c>
@@ -10642,7 +10646,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="111" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>30</v>
       </c>
@@ -10734,7 +10738,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="112" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>30</v>
       </c>
@@ -10826,7 +10830,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="113" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>30</v>
       </c>
@@ -10918,7 +10922,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="114" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>30</v>
       </c>
@@ -11010,7 +11014,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="115" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>30</v>
       </c>
@@ -11102,7 +11106,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="116" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>30</v>
       </c>
@@ -11194,7 +11198,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="117" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>30</v>
       </c>
@@ -11286,7 +11290,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="118" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>30</v>
       </c>
@@ -11378,7 +11382,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="119" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>30</v>
       </c>
@@ -11470,7 +11474,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="120" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>30</v>
       </c>
@@ -11562,7 +11566,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="121" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>30</v>
       </c>
@@ -11654,7 +11658,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="122" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>30</v>
       </c>
@@ -11746,7 +11750,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="123" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>30</v>
       </c>
@@ -11838,7 +11842,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="124" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>30</v>
       </c>
@@ -11930,7 +11934,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="125" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>30</v>
       </c>
@@ -12022,7 +12026,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="126" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>30</v>
       </c>
@@ -12114,7 +12118,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="127" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>30</v>
       </c>
@@ -12206,7 +12210,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="128" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>30</v>
       </c>
@@ -12298,7 +12302,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="129" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>30</v>
       </c>
@@ -12390,7 +12394,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="130" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>30</v>
       </c>
@@ -12574,7 +12578,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="132" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>30</v>
       </c>
@@ -12758,7 +12762,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="134" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>30</v>
       </c>
@@ -12942,7 +12946,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="136" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>30</v>
       </c>
@@ -13126,7 +13130,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="138" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>30</v>
       </c>
@@ -13310,7 +13314,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="140" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>30</v>
       </c>
@@ -13494,7 +13498,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="142" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>30</v>
       </c>
@@ -13678,7 +13682,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="144" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>30</v>
       </c>
@@ -13862,7 +13866,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="146" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>30</v>
       </c>
@@ -14046,7 +14050,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="148" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>30</v>
       </c>
@@ -14230,7 +14234,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="150" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>30</v>
       </c>
@@ -14414,7 +14418,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="152" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>30</v>
       </c>
@@ -14598,7 +14602,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="154" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>30</v>
       </c>
@@ -14782,7 +14786,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="156" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>30</v>
       </c>
@@ -14966,7 +14970,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="158" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>30</v>
       </c>
@@ -15150,7 +15154,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="160" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>30</v>
       </c>
@@ -15334,7 +15338,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="162" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>30</v>
       </c>
@@ -15518,7 +15522,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="164" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>30</v>
       </c>
@@ -15702,7 +15706,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="166" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>30</v>
       </c>
@@ -15886,7 +15890,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="168" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>30</v>
       </c>
@@ -16070,7 +16074,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="170" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>30</v>
       </c>
@@ -16254,7 +16258,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="172" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>30</v>
       </c>
@@ -16438,7 +16442,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="174" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>30</v>
       </c>
@@ -16622,7 +16626,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="176" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>30</v>
       </c>
@@ -16806,7 +16810,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="178" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>30</v>
       </c>
@@ -16990,7 +16994,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="180" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>30</v>
       </c>
@@ -17174,7 +17178,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="182" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>30</v>
       </c>
@@ -17358,7 +17362,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="184" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>30</v>
       </c>
@@ -17542,7 +17546,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="186" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>30</v>
       </c>
@@ -17726,7 +17730,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="188" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>30</v>
       </c>
@@ -17910,7 +17914,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="190" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>30</v>
       </c>
@@ -18094,7 +18098,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="192" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>30</v>
       </c>
@@ -18278,7 +18282,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="194" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>30</v>
       </c>
@@ -18462,7 +18466,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="196" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>30</v>
       </c>
@@ -18646,7 +18650,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="198" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>30</v>
       </c>
@@ -18830,7 +18834,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="200" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>30</v>
       </c>
@@ -19014,7 +19018,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="202" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>30</v>
       </c>
@@ -19198,7 +19202,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="204" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>30</v>
       </c>
@@ -19382,7 +19386,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="206" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>30</v>
       </c>
@@ -19566,7 +19570,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="208" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>30</v>
       </c>
@@ -19750,7 +19754,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="210" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>30</v>
       </c>
@@ -19934,7 +19938,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="212" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>30</v>
       </c>
@@ -20118,7 +20122,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="214" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>30</v>
       </c>
@@ -20302,7 +20306,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="216" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>30</v>
       </c>
@@ -20486,7 +20490,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="218" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>30</v>
       </c>
@@ -20670,7 +20674,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="220" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>30</v>
       </c>
@@ -20854,7 +20858,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="222" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>30</v>
       </c>
@@ -21038,7 +21042,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="224" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>30</v>
       </c>
@@ -21222,7 +21226,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="226" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>30</v>
       </c>
@@ -21406,7 +21410,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="228" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>30</v>
       </c>
@@ -21590,7 +21594,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="230" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>30</v>
       </c>
@@ -21774,7 +21778,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="232" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>30</v>
       </c>
@@ -21958,7 +21962,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="234" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>30</v>
       </c>
@@ -22142,7 +22146,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="236" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>30</v>
       </c>
@@ -22326,7 +22330,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="238" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>30</v>
       </c>
@@ -22510,7 +22514,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="240" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>30</v>
       </c>
@@ -22694,7 +22698,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="242" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>30</v>
       </c>
@@ -22878,7 +22882,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="244" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>30</v>
       </c>
@@ -23062,7 +23066,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="246" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>30</v>
       </c>
@@ -23246,7 +23250,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="248" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>30</v>
       </c>
@@ -23430,7 +23434,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="250" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>30</v>
       </c>
@@ -23614,7 +23618,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>30</v>
       </c>
@@ -23798,7 +23802,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>30</v>
       </c>
@@ -23982,7 +23986,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>30</v>
       </c>
@@ -24166,7 +24170,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="258" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>40</v>
       </c>
@@ -24258,7 +24262,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="259" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>40</v>
       </c>
@@ -24350,7 +24354,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="260" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>40</v>
       </c>
@@ -24442,7 +24446,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="261" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>40</v>
       </c>
@@ -24534,7 +24538,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="262" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>40</v>
       </c>
@@ -24626,7 +24630,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="263" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>40</v>
       </c>
@@ -24718,7 +24722,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="264" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>40</v>
       </c>
@@ -24810,7 +24814,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="265" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>40</v>
       </c>
@@ -24902,7 +24906,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="266" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>40</v>
       </c>
@@ -24994,7 +24998,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="267" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>40</v>
       </c>
@@ -25086,7 +25090,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="268" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>40</v>
       </c>
@@ -25178,7 +25182,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="269" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>40</v>
       </c>
@@ -25270,7 +25274,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="270" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>40</v>
       </c>
@@ -25362,7 +25366,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="271" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>40</v>
       </c>
@@ -25454,7 +25458,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="272" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>40</v>
       </c>
@@ -25546,7 +25550,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="273" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>40</v>
       </c>
@@ -25638,7 +25642,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="274" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>40</v>
       </c>
@@ -25730,7 +25734,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="275" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>40</v>
       </c>
@@ -25822,7 +25826,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="276" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>40</v>
       </c>
@@ -25914,7 +25918,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="277" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>40</v>
       </c>
@@ -26006,7 +26010,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="278" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>40</v>
       </c>
@@ -26098,7 +26102,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="279" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>40</v>
       </c>
@@ -26190,7 +26194,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="280" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>40</v>
       </c>
@@ -26282,7 +26286,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="281" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>40</v>
       </c>
@@ -26374,7 +26378,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="282" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>40</v>
       </c>
@@ -26466,7 +26470,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="283" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>40</v>
       </c>
@@ -26558,7 +26562,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="284" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>40</v>
       </c>
@@ -26650,7 +26654,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="285" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>40</v>
       </c>
@@ -26742,7 +26746,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="286" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>40</v>
       </c>
@@ -26834,7 +26838,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="287" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>40</v>
       </c>
@@ -26926,7 +26930,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="288" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>40</v>
       </c>
@@ -27018,7 +27022,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="289" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>40</v>
       </c>
@@ -27110,7 +27114,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="290" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>40</v>
       </c>
@@ -27202,7 +27206,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="291" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>40</v>
       </c>
@@ -27294,7 +27298,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="292" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>40</v>
       </c>
@@ -27386,7 +27390,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="293" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>40</v>
       </c>
@@ -27478,7 +27482,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="294" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>40</v>
       </c>
@@ -27570,7 +27574,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="295" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>40</v>
       </c>
@@ -27662,7 +27666,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="296" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>40</v>
       </c>
@@ -27754,7 +27758,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="297" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>40</v>
       </c>
@@ -27846,7 +27850,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="298" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>40</v>
       </c>
@@ -27938,7 +27942,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="299" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>40</v>
       </c>
@@ -28030,7 +28034,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="300" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>40</v>
       </c>
@@ -28122,7 +28126,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="301" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>40</v>
       </c>
@@ -28214,7 +28218,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="302" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>40</v>
       </c>
@@ -28306,7 +28310,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="303" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>40</v>
       </c>
@@ -28398,7 +28402,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="304" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>40</v>
       </c>
@@ -28490,7 +28494,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="305" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>40</v>
       </c>
@@ -28582,7 +28586,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="306" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>40</v>
       </c>
@@ -28674,7 +28678,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="307" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>40</v>
       </c>
@@ -28766,7 +28770,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="308" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>40</v>
       </c>
@@ -28858,7 +28862,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="309" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>40</v>
       </c>
@@ -28950,7 +28954,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="310" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>40</v>
       </c>
@@ -29042,7 +29046,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="311" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>40</v>
       </c>
@@ -29134,7 +29138,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="312" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>40</v>
       </c>
@@ -29226,7 +29230,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="313" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>40</v>
       </c>
@@ -29318,7 +29322,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="314" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>40</v>
       </c>
@@ -29410,7 +29414,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="315" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>40</v>
       </c>
@@ -29502,7 +29506,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="316" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>40</v>
       </c>
@@ -29594,7 +29598,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="317" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>40</v>
       </c>
@@ -29686,7 +29690,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="318" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>40</v>
       </c>
@@ -29778,7 +29782,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="319" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>40</v>
       </c>
@@ -29870,7 +29874,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="320" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>40</v>
       </c>
@@ -29962,7 +29966,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="321" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>40</v>
       </c>
@@ -30054,7 +30058,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="322" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>40</v>
       </c>
@@ -30146,7 +30150,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="323" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>40</v>
       </c>
@@ -30238,7 +30242,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="324" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>40</v>
       </c>
@@ -30330,7 +30334,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="325" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>40</v>
       </c>
@@ -30422,7 +30426,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="326" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>40</v>
       </c>
@@ -30514,7 +30518,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="327" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>40</v>
       </c>
@@ -30606,7 +30610,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="328" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>40</v>
       </c>
@@ -30698,7 +30702,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="329" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>40</v>
       </c>
@@ -30790,7 +30794,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="330" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>40</v>
       </c>
@@ -30882,7 +30886,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="331" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>40</v>
       </c>
@@ -30974,7 +30978,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="332" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>40</v>
       </c>
@@ -31066,7 +31070,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="333" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>40</v>
       </c>
@@ -31158,7 +31162,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="334" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>40</v>
       </c>
@@ -31250,7 +31254,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="335" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>40</v>
       </c>
@@ -31342,7 +31346,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="336" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>40</v>
       </c>
@@ -31434,7 +31438,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="337" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>40</v>
       </c>
@@ -31526,7 +31530,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="338" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>40</v>
       </c>
@@ -31618,7 +31622,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="339" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>40</v>
       </c>
@@ -31710,7 +31714,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="340" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>40</v>
       </c>
@@ -31802,7 +31806,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="341" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>40</v>
       </c>
@@ -31894,7 +31898,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="342" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>40</v>
       </c>
@@ -31986,7 +31990,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="343" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>40</v>
       </c>
@@ -32078,7 +32082,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="344" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>40</v>
       </c>
@@ -32170,7 +32174,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="345" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>40</v>
       </c>
@@ -32262,7 +32266,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="346" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>40</v>
       </c>
@@ -32354,7 +32358,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="347" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>40</v>
       </c>
@@ -32446,7 +32450,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="348" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>40</v>
       </c>
@@ -32538,7 +32542,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="349" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>40</v>
       </c>
@@ -32630,7 +32634,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="350" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>40</v>
       </c>
@@ -32722,7 +32726,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="351" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>40</v>
       </c>
@@ -32814,7 +32818,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="352" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>40</v>
       </c>
@@ -32906,7 +32910,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="353" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>40</v>
       </c>
@@ -32998,7 +33002,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="354" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>40</v>
       </c>
@@ -33090,7 +33094,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="355" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>40</v>
       </c>
@@ -33182,7 +33186,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="356" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>40</v>
       </c>
@@ -33274,7 +33278,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="357" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>40</v>
       </c>
@@ -33366,7 +33370,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="358" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>40</v>
       </c>
@@ -33458,7 +33462,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="359" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>40</v>
       </c>
@@ -33550,7 +33554,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="360" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>40</v>
       </c>
@@ -33642,7 +33646,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="361" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>40</v>
       </c>
@@ -33734,7 +33738,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="362" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>40</v>
       </c>
@@ -33826,7 +33830,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="363" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>40</v>
       </c>
@@ -33918,7 +33922,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="364" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>40</v>
       </c>
@@ -34010,7 +34014,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="365" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>40</v>
       </c>
@@ -34102,7 +34106,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="366" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>40</v>
       </c>
@@ -34194,7 +34198,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="367" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>40</v>
       </c>
@@ -34286,7 +34290,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="368" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>40</v>
       </c>
@@ -34378,7 +34382,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="369" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>40</v>
       </c>
@@ -34470,7 +34474,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="370" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>40</v>
       </c>
@@ -34562,7 +34566,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="371" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>40</v>
       </c>
@@ -34654,7 +34658,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="372" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>40</v>
       </c>
@@ -34746,7 +34750,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="373" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>40</v>
       </c>
@@ -34838,7 +34842,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="374" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>40</v>
       </c>
@@ -34930,7 +34934,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="375" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>40</v>
       </c>
@@ -35022,7 +35026,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="376" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>40</v>
       </c>
@@ -35114,7 +35118,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="377" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>40</v>
       </c>
@@ -35206,7 +35210,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="378" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>40</v>
       </c>
@@ -35298,7 +35302,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="379" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>40</v>
       </c>
@@ -35390,7 +35394,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="380" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>40</v>
       </c>
@@ -35482,7 +35486,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="381" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>40</v>
       </c>
@@ -35574,7 +35578,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="382" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>40</v>
       </c>
@@ -35666,7 +35670,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="383" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>40</v>
       </c>
@@ -35758,7 +35762,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="384" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>40</v>
       </c>
@@ -35850,7 +35854,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="385" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>40</v>
       </c>
@@ -35942,7 +35946,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="386" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>40</v>
       </c>
@@ -36126,7 +36130,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="388" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>40</v>
       </c>
@@ -36310,7 +36314,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="390" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>40</v>
       </c>
@@ -36494,7 +36498,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="392" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>40</v>
       </c>
@@ -36678,7 +36682,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="394" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>40</v>
       </c>
@@ -36862,7 +36866,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="396" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>40</v>
       </c>
@@ -37046,7 +37050,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="398" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>40</v>
       </c>
@@ -37230,7 +37234,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="400" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>40</v>
       </c>
@@ -37414,7 +37418,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="402" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>40</v>
       </c>
@@ -37598,7 +37602,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="404" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>40</v>
       </c>
@@ -37782,7 +37786,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="406" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>40</v>
       </c>
@@ -37966,7 +37970,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="408" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>40</v>
       </c>
@@ -38150,7 +38154,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="410" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>40</v>
       </c>
@@ -38334,7 +38338,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="412" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>40</v>
       </c>
@@ -38518,7 +38522,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="414" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>40</v>
       </c>
@@ -38702,7 +38706,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="416" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>40</v>
       </c>
@@ -38886,7 +38890,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="418" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>40</v>
       </c>
@@ -39070,7 +39074,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="420" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>40</v>
       </c>
@@ -39254,7 +39258,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="422" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>40</v>
       </c>
@@ -39438,7 +39442,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="424" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>40</v>
       </c>
@@ -39622,7 +39626,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="426" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>40</v>
       </c>
@@ -39806,7 +39810,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="428" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>40</v>
       </c>
@@ -39990,7 +39994,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="430" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>40</v>
       </c>
@@ -40174,7 +40178,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="432" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>40</v>
       </c>
@@ -40358,7 +40362,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="434" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>40</v>
       </c>
@@ -40542,7 +40546,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="436" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>40</v>
       </c>
@@ -40726,7 +40730,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="438" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>40</v>
       </c>
@@ -40910,7 +40914,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="440" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>40</v>
       </c>
@@ -41094,7 +41098,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="442" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>40</v>
       </c>
@@ -41278,7 +41282,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="444" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>40</v>
       </c>
@@ -41462,7 +41466,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="446" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>40</v>
       </c>
@@ -41646,7 +41650,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="448" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>40</v>
       </c>
@@ -41830,7 +41834,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="450" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>40</v>
       </c>
@@ -42014,7 +42018,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="452" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>40</v>
       </c>
@@ -42198,7 +42202,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="454" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>40</v>
       </c>
@@ -42382,7 +42386,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="456" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>40</v>
       </c>
@@ -42566,7 +42570,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="458" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>40</v>
       </c>
@@ -42750,7 +42754,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="460" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
         <v>40</v>
       </c>
@@ -42934,7 +42938,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="462" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>40</v>
       </c>
@@ -43118,7 +43122,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="464" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
         <v>40</v>
       </c>
@@ -43302,7 +43306,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="466" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>40</v>
       </c>
@@ -43486,7 +43490,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="468" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>40</v>
       </c>
@@ -43670,7 +43674,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="470" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
         <v>40</v>
       </c>
@@ -43854,7 +43858,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="472" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
         <v>40</v>
       </c>
@@ -44038,7 +44042,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="474" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>40</v>
       </c>
@@ -44222,7 +44226,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="476" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>40</v>
       </c>
@@ -44406,7 +44410,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="478" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>40</v>
       </c>
@@ -44590,7 +44594,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="480" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>40</v>
       </c>
@@ -44774,7 +44778,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="482" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>40</v>
       </c>
@@ -44958,7 +44962,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="484" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>40</v>
       </c>
@@ -45142,7 +45146,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="486" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>40</v>
       </c>
@@ -45326,7 +45330,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="488" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>40</v>
       </c>
@@ -45510,7 +45514,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="490" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
         <v>40</v>
       </c>
@@ -45694,7 +45698,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="492" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
         <v>40</v>
       </c>
@@ -45878,7 +45882,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="494" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
         <v>40</v>
       </c>
@@ -46062,7 +46066,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="496" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
         <v>40</v>
       </c>
@@ -46246,7 +46250,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="498" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
         <v>40</v>
       </c>
@@ -46430,7 +46434,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="500" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
         <v>40</v>
       </c>
@@ -46614,7 +46618,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="502" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
         <v>40</v>
       </c>
@@ -46798,7 +46802,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="504" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
         <v>40</v>
       </c>
@@ -46982,7 +46986,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="506" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
         <v>40</v>
       </c>
@@ -47166,7 +47170,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="508" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
         <v>40</v>
       </c>
@@ -47350,7 +47354,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="510" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
         <v>40</v>
       </c>
@@ -47534,7 +47538,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="512" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
         <v>40</v>
       </c>
@@ -47719,6 +47723,18 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AD513" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="nn"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <filters>
+        <filter val="AdaSyn"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>